<commit_message>
Enviado el 17 de abril
</commit_message>
<xml_diff>
--- a/Api.xlsx
+++ b/Api.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ControWell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0FF267-7FCA-40AE-8A34-45F293552506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A155E1A-7B38-42A0-85E6-C6B4E903C339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-2070" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Controladores" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>Controlador</t>
   </si>
@@ -78,6 +78,39 @@
   </si>
   <si>
     <t>BalanceRespuesta = await respuestajson.Content.ReadFromJsonAsync&lt;Balance&gt;();</t>
+  </si>
+  <si>
+    <t>Rango</t>
+  </si>
+  <si>
+    <t>Balances dentro de un rango de fechas</t>
+  </si>
+  <si>
+    <t>Consulta</t>
+  </si>
+  <si>
+    <t>var resultado = await Http.PostAsJsonAsync("api/Balance/Rango", consultaBal);</t>
+  </si>
+  <si>
+    <t>Listado = await resultado.Content.ReadFromJsonAsync&lt;List&lt;Balance&gt;&gt;();</t>
+  </si>
+  <si>
+    <t>List&lt;Balance&gt;</t>
+  </si>
+  <si>
+    <t>Traer listado de tanques</t>
+  </si>
+  <si>
+    <t>HttpGet</t>
+  </si>
+  <si>
+    <t>List&lt;Tanque&gt;</t>
+  </si>
+  <si>
+    <t>Tanque</t>
+  </si>
+  <si>
+    <t>var resultado = await Http.GetFromJsonAsync&lt;List&lt;Tanque&gt;&gt;("api/Tanque");</t>
   </si>
 </sst>
 </file>
@@ -395,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,6 +522,49 @@
       </c>
       <c r="H3" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>